<commit_message>
apply fixed texts of previous commits (Kilian) to ids_questionnaire
</commit_message>
<xml_diff>
--- a/data_raw/ids_questionnaire.xlsx
+++ b/data_raw/ids_questionnaire.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" state="visible" r:id="rId2"/>
@@ -1476,7 +1476,7 @@
     <t xml:space="preserve">TTOI_0004_I_0001_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Wenn ich weiß, dass ich eine Aufgabe nicht gut machen kann, mache ich sie eher nicht. Auch wenn ich vielleicht dabei viel lernen würde.</t>
+    <t xml:space="preserve">Wenn ich weiß, dass ich eine Aufgabe nicht gut machen kann, mache ich sie eher nicht, auch wenn ich vielleicht dabei viel lernen würde.</t>
   </si>
   <si>
     <t xml:space="preserve">If I knew I wasn't going to do well at a task, I probably wouldn't do it even if I might learn a lot from it.</t>
@@ -3181,7 +3181,7 @@
     <t xml:space="preserve">TPAC_0002_I_0001_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Wie oft warst du während der letzten drei Monaten aktiv beim Sportunterricht dabei (viel mitgespielt, gelaufen, gesprungen, geworfen)?</t>
+    <t xml:space="preserve">Wie oft warst du während der letzten drei Monate aktiv beim Sportunterricht dabei (viel mitgespielt, gelaufen, gesprungen, geworfen)?</t>
   </si>
   <si>
     <t xml:space="preserve">In the last three months during your physical education (PE) classes, how often were you very active (playing hard, running, jumping, throwing)? </t>
@@ -4231,7 +4231,7 @@
     <t xml:space="preserve">TSEM_0022_I_0001_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Wie oft versuchst du, was du gelernt hast mit anderen Dingen, die du kennst, zu verknüpfen?</t>
+    <t xml:space="preserve">Wie oft versuchst du, was du gelernt hast, mit anderen Dingen, die du kennst, zu verknüpfen?</t>
   </si>
   <si>
     <t xml:space="preserve">How often do you try to relate what you are studying to other things you know about?</t>
@@ -4531,7 +4531,7 @@
     <t xml:space="preserve">TSES_0007_I_0001_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Bitte kreuze nun an, welche Beschreibung am besten auf den Beruf der Person zutrifft. Arbeit die Person im Moment nicht, dann denke an die letzte Arbeitsstelle. </t>
+    <t xml:space="preserve">Bitte kreuze nun an, welche Beschreibung am besten auf den Beruf der Person zutrifft. Arbeitet die Person im Moment nicht, dann denke an die letzte Arbeitsstelle. </t>
   </si>
   <si>
     <t xml:space="preserve">Please tick one box only to best describe the work the main earner does. If the main earner is not currently working, please tick the box that best describes what his/her last job was.</t>
@@ -5331,7 +5331,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5421,10 +5421,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7940,14 +7936,14 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="96.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="96.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.58"/>
   </cols>
   <sheetData>
@@ -7968,7 +7964,7 @@
       <c r="A2" s="1" t="s">
         <v>935</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>936</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -8271,14 +8267,14 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="71"/>
   </cols>
   <sheetData>
@@ -8672,9 +8668,9 @@
       <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.59"/>
   </cols>
@@ -9114,7 +9110,7 @@
       <c r="A40" s="0" t="s">
         <v>1138</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="25" t="s">
         <v>1139</v>
       </c>
       <c r="C40" s="0" t="s">
@@ -9286,7 +9282,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.41"/>
@@ -9901,12 +9897,12 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.58"/>
@@ -10207,7 +10203,7 @@
       <c r="A27" s="0" t="s">
         <v>1326</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>1327</v>
       </c>
       <c r="C27" s="0" t="s">
@@ -10478,7 +10474,7 @@
       <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70"/>
@@ -10839,10 +10835,10 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="125.58"/>
@@ -11150,7 +11146,7 @@
       <c r="C30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="27"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11178,9 +11174,9 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="57.41"/>
   </cols>
@@ -11205,7 +11201,7 @@
       <c r="B2" s="1" t="s">
         <v>1489</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>1490</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -11219,7 +11215,7 @@
       <c r="B3" s="1" t="s">
         <v>1492</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>1493</v>
       </c>
     </row>
@@ -11241,7 +11237,7 @@
       <c r="B5" s="8" t="s">
         <v>1496</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>1497</v>
       </c>
     </row>
@@ -11263,7 +11259,7 @@
       <c r="B7" s="1" t="s">
         <v>1500</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>1501</v>
       </c>
     </row>
@@ -11285,7 +11281,7 @@
       <c r="B9" s="1" t="s">
         <v>1504</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>1505</v>
       </c>
     </row>
@@ -11307,7 +11303,7 @@
       <c r="B11" s="1" t="s">
         <v>1508</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>1509</v>
       </c>
     </row>
@@ -11329,7 +11325,7 @@
       <c r="B13" s="1" t="s">
         <v>1512</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>1513</v>
       </c>
     </row>
@@ -11351,7 +11347,7 @@
       <c r="B15" s="1" t="s">
         <v>1516</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>1517</v>
       </c>
     </row>
@@ -11373,7 +11369,7 @@
       <c r="B17" s="1" t="s">
         <v>1520</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>1521</v>
       </c>
     </row>
@@ -11395,7 +11391,7 @@
       <c r="B19" s="1" t="s">
         <v>1524</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>1525</v>
       </c>
     </row>
@@ -11417,7 +11413,7 @@
       <c r="B21" s="1" t="s">
         <v>1528</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>1529</v>
       </c>
     </row>
@@ -11461,11 +11457,11 @@
   </sheetPr>
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C63" activeCellId="0" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.5"/>
@@ -12226,7 +12222,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.5"/>
@@ -12463,7 +12459,7 @@
       <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="72.42"/>
@@ -12656,7 +12652,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="89.58"/>
@@ -13057,9 +13053,9 @@
       <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="98.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="47.92"/>
@@ -13543,11 +13539,11 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="105.09"/>
@@ -13880,7 +13876,7 @@
       <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.08"/>
@@ -14211,7 +14207,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="60"/>
@@ -14540,11 +14536,11 @@
       <selection pane="topLeft" activeCell="C124" activeCellId="0" sqref="C124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.92"/>
   </cols>
@@ -14834,7 +14830,7 @@
       <c r="B24" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="4" t="s">
         <v>654</v>
       </c>
     </row>
@@ -14858,7 +14854,7 @@
       <c r="B26" s="4" t="s">
         <v>657</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="4" t="s">
         <v>658</v>
       </c>
     </row>
@@ -14882,7 +14878,7 @@
       <c r="B28" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="4" t="s">
         <v>662</v>
       </c>
     </row>
@@ -14906,7 +14902,7 @@
       <c r="B30" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="4" t="s">
         <v>666</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -15005,7 +15001,7 @@
       <c r="B38" s="4" t="s">
         <v>680</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="4" t="s">
         <v>681</v>
       </c>
     </row>
@@ -15029,7 +15025,7 @@
       <c r="B40" s="4" t="s">
         <v>684</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="4" t="s">
         <v>685</v>
       </c>
     </row>
@@ -15053,7 +15049,7 @@
       <c r="B42" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="4" t="s">
         <v>689</v>
       </c>
     </row>
@@ -15077,7 +15073,7 @@
       <c r="B44" s="6" t="s">
         <v>692</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="4" t="s">
         <v>693</v>
       </c>
     </row>
@@ -15101,7 +15097,7 @@
       <c r="B46" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="4" t="s">
         <v>697</v>
       </c>
       <c r="D46" s="4" t="s">
@@ -15200,7 +15196,7 @@
       <c r="B54" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C54" s="23" t="s">
+      <c r="C54" s="4" t="s">
         <v>712</v>
       </c>
       <c r="D54" s="4" t="s">
@@ -16547,7 +16543,7 @@
       <c r="A163" s="4" t="s">
         <v>928</v>
       </c>
-      <c r="B163" s="24" t="s">
+      <c r="B163" s="23" t="s">
         <v>129</v>
       </c>
       <c r="C163" s="1" t="s">

</xml_diff>